<commit_message>
feat: cambio en los totales para sumar el no remunerativo
</commit_message>
<xml_diff>
--- a/public/importar-ejemplo.xlsx
+++ b/public/importar-ejemplo.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7507DE0F-6AAA-4B94-B1F3-6947D9F79B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Escritorio\Lumar\uesevi-app\public\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A79E9EC-FADD-48D1-9268-CE02A376C072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Nombre</t>
   </si>
@@ -77,13 +82,16 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Suma no remunerativa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -258,9 +266,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,7 +306,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -404,7 +412,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -546,7 +554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,13 +562,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="14.5703125" style="1"/>
     <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
@@ -568,9 +576,10 @@
     <col min="6" max="7" width="14.5703125" style="1"/>
     <col min="8" max="1013" width="14.5703125" hidden="1"/>
     <col min="1014" max="1024" width="11.5703125" hidden="1" customWidth="1"/>
+    <col min="1025" max="1025" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7 1025:1025" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -592,8 +601,11 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="AMK1" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7 1025:1025" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -615,8 +627,11 @@
       <c r="G2" s="1">
         <v>15000</v>
       </c>
+      <c r="AMK2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7 1025:1025" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -637,6 +652,9 @@
       </c>
       <c r="G3" s="1">
         <v>0</v>
+      </c>
+      <c r="AMK3" s="1">
+        <v>15000</v>
       </c>
     </row>
   </sheetData>
@@ -651,6 +669,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: cambio para usar la suma no remunerativa
</commit_message>
<xml_diff>
--- a/public/importar-ejemplo.xlsx
+++ b/public/importar-ejemplo.xlsx
@@ -41,7 +41,7 @@
     <t>Adicionales</t>
   </si>
   <si>
-    <t>Ad. Remunerativo</t>
+    <t>Suma no remunerativa</t>
   </si>
   <si>
     <t>Juan</t>
@@ -2560,7 +2560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>26280</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>

</xml_diff>